<commit_message>
Upload ballParam and ball prefabs
</commit_message>
<xml_diff>
--- a/LubanConfig/DataTables/Datas/#BallParam.xlsx
+++ b/LubanConfig/DataTables/Datas/#BallParam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\monster-ball\LubanConfig\DataTables\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C86B66D-DB82-4CA3-BD92-C737049357B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148E4185-8CD4-45A5-9117-40BAAADE28F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BallParam" sheetId="1" r:id="rId1"/>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>##var</t>
   </si>
@@ -293,12 +293,32 @@
     <t>float</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>AssetID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fireball</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ball</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Splitball</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -325,6 +345,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -346,12 +373,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -576,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -618,7 +648,9 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -671,7 +703,9 @@
       <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -786,6 +820,9 @@
       <c r="K5" s="1">
         <v>80</v>
       </c>
+      <c r="L5" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -819,7 +856,9 @@
       <c r="K6" s="1">
         <v>60</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -870,7 +909,9 @@
       <c r="K7" s="1">
         <v>40</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -921,7 +962,9 @@
       <c r="K8" s="1">
         <v>35</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -966,9 +1009,15 @@
       <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="J9" s="1">
+        <v>300</v>
+      </c>
+      <c r="K9" s="1">
+        <v>60</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>

</xml_diff>